<commit_message>
Doc: updated Bugs status to closed
</commit_message>
<xml_diff>
--- a/Test/Bug-Report.xlsx
+++ b/Test/Bug-Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Online-Mobile-Store-WebSite\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C6D909-DC7F-4642-95DF-D6682D979142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFA411D-6860-4007-8BBC-B3934F581048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Abdallah</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Development</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
 2. Fill in all fields with valid data except User Type
 3. Leave User Type unselected
 4. Click "Register"</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,72 +591,72 @@
     </row>
     <row r="2" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
         <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Bugs to Bug Report
</commit_message>
<xml_diff>
--- a/Test/Bug-Report.xlsx
+++ b/Test/Bug-Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online-Mobile-Store-WebSite\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFA411D-6860-4007-8BBC-B3934F581048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F17CB43-6CEB-4B3D-81C4-1E77C4A6A03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Title</t>
   </si>
@@ -109,6 +109,27 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>Bug_Client_001</t>
+  </si>
+  <si>
+    <t>TC_Client_017</t>
+  </si>
+  <si>
+    <t>Empty cart message not appear</t>
+  </si>
+  <si>
+    <t>no message appear</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> message: "Your cart is empty"</t>
+  </si>
+  <si>
+    <t>1. Login with Client email
+2.  Navigate to Home page 
+3. Click on Cart Button
+4. Message will appear</t>
   </si>
 </sst>
 </file>
@@ -533,28 +554,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.453125" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.54296875" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -589,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -624,7 +645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -656,6 +677,41 @@
         <v>11</v>
       </c>
       <c r="K3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Doc: Updated bugs status to closed as this bugs are fixed
</commit_message>
<xml_diff>
--- a/Test/Bug-Report.xlsx
+++ b/Test/Bug-Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Online-Mobile-Store-WebSite\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB27147B-35F2-464F-B458-8F6FD83139A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8335A87-9E14-42C3-966E-C7B66332A793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Title</t>
   </si>
@@ -141,9 +141,6 @@
     <t>1. Type "1234567890123" in National ID field
 2. Fill other fields with valid data
 3. Click "Register"</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Registration Successful</t>
@@ -217,40 +214,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -268,61 +237,31 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,212 +567,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
-        <v>35</v>
+      <c r="K4" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="5" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>